<commit_message>
running all Profile xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="128">
   <si>
     <t>TCID</t>
   </si>
@@ -485,9 +485,6 @@
   </si>
   <si>
     <t>Profile40</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -911,7 +908,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D41"/>
+      <selection activeCell="D2" sqref="D2:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -968,7 +965,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>51</v>
@@ -985,7 +982,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>51</v>
@@ -1002,7 +999,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>51</v>
@@ -1019,7 +1016,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>51</v>
@@ -1036,7 +1033,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>51</v>
@@ -1053,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>51</v>
@@ -1070,7 +1067,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>51</v>
@@ -1087,7 +1084,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>51</v>
@@ -1104,7 +1101,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>51</v>
@@ -1121,7 +1118,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>51</v>
@@ -1138,7 +1135,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>51</v>
@@ -1155,7 +1152,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>51</v>
@@ -1172,7 +1169,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>51</v>
@@ -1189,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>51</v>
@@ -1206,7 +1203,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>51</v>
@@ -1223,7 +1220,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>51</v>
@@ -1240,7 +1237,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>51</v>
@@ -1257,7 +1254,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>51</v>
@@ -1274,7 +1271,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>51</v>
@@ -1291,7 +1288,7 @@
         <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>51</v>
@@ -1308,7 +1305,7 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>51</v>
@@ -1325,7 +1322,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>51</v>
@@ -1342,7 +1339,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>51</v>
@@ -1359,7 +1356,7 @@
         <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>51</v>
@@ -1376,7 +1373,7 @@
         <v>57</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>51</v>
@@ -1393,7 +1390,7 @@
         <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>51</v>
@@ -1410,7 +1407,7 @@
         <v>59</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>51</v>
@@ -1427,7 +1424,7 @@
         <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>51</v>
@@ -1444,7 +1441,7 @@
         <v>65</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>51</v>
@@ -1461,7 +1458,7 @@
         <v>66</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>51</v>
@@ -1478,7 +1475,7 @@
         <v>67</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>51</v>
@@ -1495,7 +1492,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>51</v>
@@ -1512,7 +1509,7 @@
         <v>69</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>51</v>
@@ -1529,7 +1526,7 @@
         <v>70</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>51</v>
@@ -1546,7 +1543,7 @@
         <v>71</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>51</v>
@@ -1563,7 +1560,7 @@
         <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>51</v>
@@ -1580,7 +1577,7 @@
         <v>73</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>51</v>
@@ -1597,7 +1594,7 @@
         <v>74</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>51</v>
@@ -1614,7 +1611,7 @@
         <v>75</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Adding new profile script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="131">
   <si>
     <t>TCID</t>
   </si>
@@ -485,6 +485,15 @@
   </si>
   <si>
     <t>Profile40</t>
+  </si>
+  <si>
+    <t>Profile41</t>
+  </si>
+  <si>
+    <t>Verify that HCR having Badge append with his name in Profile page</t>
+  </si>
+  <si>
+    <t>OPQA-2726</t>
   </si>
 </sst>
 </file>
@@ -905,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1617,9 +1626,27 @@
         <v>55</v>
       </c>
     </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="8"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added New Profile script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
   <si>
     <t>TCID</t>
   </si>
@@ -494,6 +494,15 @@
   </si>
   <si>
     <t>OPQA-2726</t>
+  </si>
+  <si>
+    <t>Verify that user is able to edit first name and last name from his own profile page.</t>
+  </si>
+  <si>
+    <t>OPQA-2679</t>
+  </si>
+  <si>
+    <t>Profile42</t>
   </si>
 </sst>
 </file>
@@ -914,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1641,12 +1650,28 @@
       </c>
       <c r="E42" s="8"/>
     </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>
+    <hyperlink ref="B43" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2679"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed watchlist test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
   <si>
     <t>TCID</t>
   </si>
@@ -485,6 +485,24 @@
   </si>
   <si>
     <t>Profile40</t>
+  </si>
+  <si>
+    <t>Profile41</t>
+  </si>
+  <si>
+    <t>Verify that HCR having Badge append with his name in Profile page</t>
+  </si>
+  <si>
+    <t>OPQA-2726</t>
+  </si>
+  <si>
+    <t>Verify that user is able to edit first name and last name from his own profile page.</t>
+  </si>
+  <si>
+    <t>OPQA-2679</t>
+  </si>
+  <si>
+    <t>Profile42</t>
   </si>
 </sst>
 </file>
@@ -905,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1617,9 +1635,43 @@
         <v>55</v>
       </c>
     </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="8"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>
+    <hyperlink ref="B43" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2679"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
new profile script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="143">
   <si>
     <t>TCID</t>
   </si>
@@ -511,6 +511,25 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that user is able to update his first name and last name  fields with max length count </t>
+  </si>
+  <si>
+    <t>Profile44</t>
+  </si>
+  <si>
+    <t>OPQA-2936|OPQA-2939|OPQA-2938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that Profile Picture  modal window ‘update’ button should be disabled by default|Verify that Profile picture modal window should contain default buttons and messages|Verify that Profile Picture  modal window should be disappear  while click on ‘Close(X)’ button
+</t>
+  </si>
+  <si>
+    <t>Profile45</t>
+  </si>
+  <si>
+    <t>Verify that Profile Picture  modal window should be disappear  while click on ‘Cancel’ button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQA-2937 </t>
   </si>
 </sst>
 </file>
@@ -607,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -630,6 +649,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -931,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1688,6 +1710,36 @@
       </c>
       <c r="E44" s="8"/>
     </row>
+    <row r="45" spans="1:5" ht="60">
+      <c r="A45" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
script changes in profile
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -953,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1740,12 +1740,6 @@
       </c>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:5">
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="B48" s="8"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
updated Zephyr id in profile.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="146">
   <si>
     <t>TCID</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>Verify that profile call to Action(CTA) in a white box is getting  displayed in country field when your first name, last name, title/role, institution, or location/country is blank</t>
+  </si>
+  <si>
+    <t>OPQA-3251</t>
   </si>
 </sst>
 </file>
@@ -962,7 +965,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1716,7 +1719,7 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" ht="60">
+    <row r="45" spans="1:5" ht="45">
       <c r="A45" s="2" t="s">
         <v>137</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>143</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
implemented new profile test case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="149">
   <si>
     <t>TCID</t>
   </si>
@@ -539,6 +539,15 @@
   </si>
   <si>
     <t>OPQA-3251</t>
+  </si>
+  <si>
+    <t>Profile47</t>
+  </si>
+  <si>
+    <t>Verify that profile call to Action(CTA) in a white box is getting  displayed in Summary field when your profile summary is blank</t>
+  </si>
+  <si>
+    <t>OPQA-3323</t>
   </si>
 </sst>
 </file>
@@ -962,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1764,6 +1773,21 @@
       </c>
       <c r="E47" s="8"/>
     </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
profile onboarding scripts added
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
   <si>
     <t>TCID</t>
   </si>
@@ -566,12 +566,21 @@
   <si>
     <t>Profile49</t>
   </si>
+  <si>
+    <t>OPQA-2118</t>
+  </si>
+  <si>
+    <t>Profile50</t>
+  </si>
+  <si>
+    <t>Verify that system is capturing the on-boarded events.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,6 +632,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -690,7 +705,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -724,6 +739,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1026,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1873,6 +1891,21 @@
       </c>
       <c r="E50" s="8"/>
     </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
profile new script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="161">
   <si>
     <t>TCID</t>
   </si>
@@ -574,6 +574,15 @@
   </si>
   <si>
     <t>Verify that system is capturing the on-boarded events.</t>
+  </si>
+  <si>
+    <t>OPQA-2822</t>
+  </si>
+  <si>
+    <t>Profile51</t>
+  </si>
+  <si>
+    <t>Verify that deep linking is working as expected for other’s profile page using STeAM account</t>
   </si>
 </sst>
 </file>
@@ -705,7 +714,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -744,6 +753,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1044,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1906,6 +1916,21 @@
       </c>
       <c r="E51" s="8"/>
     </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
profile onboarding script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="176">
   <si>
     <t>TCID</t>
   </si>
@@ -567,9 +567,6 @@
     <t>Profile49</t>
   </si>
   <si>
-    <t>OPQA-2118</t>
-  </si>
-  <si>
     <t>Profile50</t>
   </si>
   <si>
@@ -606,9 +603,6 @@
     <t>Profile54</t>
   </si>
   <si>
-    <t>OPQA-2116</t>
-  </si>
-  <si>
     <t>Verify that user shall be marked as on-boarded if they click the 'Done' button on the profile model.</t>
   </si>
   <si>
@@ -624,10 +618,16 @@
     <t>Profile56</t>
   </si>
   <si>
-    <t>Verify that when user clicks outside of the profile model then user will be sent right to their desired location in Neon.</t>
-  </si>
-  <si>
-    <t>OPQA-2114</t>
+    <t>OPQA-2118|OPQA-2097</t>
+  </si>
+  <si>
+    <t>OPQA-2116|OPQA-2094</t>
+  </si>
+  <si>
+    <t>OPQA-2091||OPQA-2092||OPQA-2093</t>
+  </si>
+  <si>
+    <t>Verify that Neon on-boarding welcome modal displays text that welcomes the user to Project Neon.||Verify that Neon on-boarding welcome modal displays images of features in Project Neon.||Verify that Neon on-boarding welcome modal displays recommended Project Neon users.</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -799,6 +799,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1101,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:E57"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1948,13 +1951,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>157</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>51</v>
@@ -1963,13 +1966,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C52" s="18" t="s">
         <v>159</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>51</v>
@@ -1978,13 +1981,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>51</v>
@@ -1993,13 +1996,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>51</v>
@@ -2008,13 +2011,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" s="18" t="s">
         <v>167</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>51</v>
@@ -2023,30 +2026,32 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="D56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="B57" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="E57" s="8"/>
     </row>
   </sheetData>
@@ -2054,8 +2059,9 @@
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>
     <hyperlink ref="B43" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2679"/>
     <hyperlink ref="B50" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2821"/>
+    <hyperlink ref="B57" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2091"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
profile onboarding script implmentation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="185">
   <si>
     <t>TCID</t>
   </si>
@@ -647,6 +647,15 @@
   </si>
   <si>
     <t>Verify that user has the ability to update his Name from the profile modal.|Verify that profile modal displays the following fields pre-populated with values from the user's profile:Name (required field),Title/Role,Country,Skills and Interests (Topics)</t>
+  </si>
+  <si>
+    <t>Profile59</t>
+  </si>
+  <si>
+    <t>OPQA-2108</t>
+  </si>
+  <si>
+    <t>Verify that user has the ability to add and update the following information from the profile modal:Title/Role,Institution,Country,Skills and Interests (Topics)</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2095,6 +2104,21 @@
       </c>
       <c r="E59" s="8"/>
     </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
profile onboarding scripts ENW to Neon
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="197">
   <si>
     <t>TCID</t>
   </si>
@@ -665,6 +665,33 @@
   </si>
   <si>
     <t>Verify that the system records the user as on-boarded if he exits the Neon on-boarding welcome modal without clicking on the "Done" button.</t>
+  </si>
+  <si>
+    <t>Profile61</t>
+  </si>
+  <si>
+    <t>OPQA-2087</t>
+  </si>
+  <si>
+    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Project Neon" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
+  </si>
+  <si>
+    <t>OPQA-2089</t>
+  </si>
+  <si>
+    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Profile" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
+  </si>
+  <si>
+    <t>Profile62</t>
+  </si>
+  <si>
+    <t>OPQA-2090</t>
+  </si>
+  <si>
+    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Account" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
+  </si>
+  <si>
+    <t>Profile63</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2143,6 +2170,51 @@
       </c>
       <c r="E61" s="8"/>
     </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
profile ENW to Neon onboarding scripts implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="206">
   <si>
     <t>TCID</t>
   </si>
@@ -692,6 +692,33 @@
   </si>
   <si>
     <t>Profile63</t>
+  </si>
+  <si>
+    <t>Profile64</t>
+  </si>
+  <si>
+    <t>OPQA-1722</t>
+  </si>
+  <si>
+    <t>Verify that  A signed in ENW user shall be able to try to access their Feedback page via a link within the ENW header profile dropdown</t>
+  </si>
+  <si>
+    <t>Profile65</t>
+  </si>
+  <si>
+    <t>Profile66</t>
+  </si>
+  <si>
+    <t>OPQA-1715</t>
+  </si>
+  <si>
+    <t>Verify that  A signed in ENW user shall be able to try to access their Privacy page via a link within the ENW header profile dropdown.</t>
+  </si>
+  <si>
+    <t>OPQA-1718</t>
+  </si>
+  <si>
+    <t>Verify that  A signed in ENW user shall be able to try to access their Acceptable Use page via a link within the ENW header profile dropdown</t>
   </si>
 </sst>
 </file>
@@ -1158,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2215,6 +2242,51 @@
       </c>
       <c r="E64" s="8"/>
     </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
profile scripts code changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -65,9 +65,6 @@
     <t>Verify that user is able to edit  info like title/role,Primary Institution and country from his own profile</t>
   </si>
   <si>
-    <t>OPQA-494|OPQA-501</t>
-  </si>
-  <si>
     <t>OPQA-495</t>
   </si>
   <si>
@@ -115,13 +112,6 @@
   </si>
   <si>
     <t>JIRA ID</t>
-  </si>
-  <si>
-    <t>OPQA-444|OPQA-434</t>
-  </si>
-  <si>
-    <t>Verify that user is able to Start/Stop following a user from profile search results page
-Verify that user is able to search for profiles</t>
   </si>
   <si>
     <t>Verify that below Project Neon Header and Footer links working as expected
@@ -145,13 +135,7 @@
     <t>Verify that user is able to Start/Stop following a user from profile page</t>
   </si>
   <si>
-    <t>OPQA-435|OPQA-436</t>
-  </si>
-  <si>
     <t>OPQA-445</t>
-  </si>
-  <si>
-    <t>OPQA-496|OPQA-511</t>
   </si>
   <si>
     <t>Verify that user is able to post the article from profile page</t>
@@ -508,13 +492,6 @@
     <t>Profile44</t>
   </si>
   <si>
-    <t>OPQA-2936|OPQA-2939|OPQA-2938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that Profile Picture  modal window ‘update’ button should be disabled by default|Verify that Profile picture modal window should contain default buttons and messages|Verify that Profile Picture  modal window should be disappear  while click on ‘Close(X)’ button
-</t>
-  </si>
-  <si>
     <t>Profile45</t>
   </si>
   <si>
@@ -615,110 +592,133 @@
     <t>Profile56</t>
   </si>
   <si>
-    <t>OPQA-2118|OPQA-2097</t>
-  </si>
-  <si>
     <t>OPQA-2091||OPQA-2092||OPQA-2093</t>
   </si>
   <si>
     <t>Verify that Neon on-boarding welcome modal displays text that welcomes the user to Project Neon.||Verify that Neon on-boarding welcome modal displays images of features in Project Neon.||Verify that Neon on-boarding welcome modal displays recommended Project Neon users.</t>
   </si>
   <si>
-    <t>OPQA-2116|OPQA-2094|OPQA-2112</t>
-  </si>
-  <si>
-    <t>Verify that user shall be marked as on-boarded if they click the 'Done' button on the profile model.|Verify that when user clicks the 'OK' button on the Neon on-boarding welcome triggers the display of the Profile modal. | Verify that user who clicks the 'Done' button on the profile modal shall be sent to their desired location in Project Neon.</t>
-  </si>
-  <si>
     <t>Profile57</t>
   </si>
   <si>
-    <t>OPQA-2101|OPQA-2100</t>
+    <t>Profile58</t>
+  </si>
+  <si>
+    <t>Profile59</t>
+  </si>
+  <si>
+    <t>OPQA-2108</t>
+  </si>
+  <si>
+    <t>Verify that user has the ability to add and update the following information from the profile modal:Title/Role,Institution,Country,Skills and Interests (Topics)</t>
+  </si>
+  <si>
+    <t>Profile60</t>
+  </si>
+  <si>
+    <t>OPQA-2096</t>
+  </si>
+  <si>
+    <t>Verify that the system records the user as on-boarded if he exits the Neon on-boarding welcome modal without clicking on the "Done" button.</t>
+  </si>
+  <si>
+    <t>Profile61</t>
+  </si>
+  <si>
+    <t>OPQA-2087</t>
+  </si>
+  <si>
+    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Project Neon" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
+  </si>
+  <si>
+    <t>OPQA-2089</t>
+  </si>
+  <si>
+    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Profile" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
+  </si>
+  <si>
+    <t>Profile62</t>
+  </si>
+  <si>
+    <t>OPQA-2090</t>
+  </si>
+  <si>
+    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Account" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
+  </si>
+  <si>
+    <t>Profile63</t>
+  </si>
+  <si>
+    <t>Profile64</t>
+  </si>
+  <si>
+    <t>OPQA-1722</t>
+  </si>
+  <si>
+    <t>Verify that  A signed in ENW user shall be able to try to access their Feedback page via a link within the ENW header profile dropdown</t>
+  </si>
+  <si>
+    <t>Profile65</t>
+  </si>
+  <si>
+    <t>Profile66</t>
+  </si>
+  <si>
+    <t>OPQA-1715</t>
+  </si>
+  <si>
+    <t>Verify that  A signed in ENW user shall be able to try to access their Privacy page via a link within the ENW header profile dropdown.</t>
+  </si>
+  <si>
+    <t>OPQA-1718</t>
+  </si>
+  <si>
+    <t>Verify that  A signed in ENW user shall be able to try to access their Acceptable Use page via a link within the ENW header profile dropdown</t>
+  </si>
+  <si>
+    <t>OPQA-444||OPQA-434</t>
+  </si>
+  <si>
+    <t>OPQA-435||OPQA-436</t>
+  </si>
+  <si>
+    <t>OPQA-494||OPQA-501</t>
+  </si>
+  <si>
+    <t>OPQA-496||OPQA-511</t>
+  </si>
+  <si>
+    <t>OPQA-2936||OPQA-2939||OPQA-2938</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Start/Stop following a user from profile search results page ||
+Verify that user is able to search for profiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that Profile Picture  modal window ‘update’ button should be disabled by default||Verify that Profile picture modal window should contain default buttons and messages||Verify that Profile Picture  modal window should be disappear  while click on ‘Close(X)’ button
+</t>
+  </si>
+  <si>
+    <t>OPQA-2118||OPQA-2097</t>
+  </si>
+  <si>
+    <t>OPQA-2116||OPQA-2094||OPQA-2112</t>
+  </si>
+  <si>
+    <t>Verify that user shall be marked as on-boarded if they click the 'Done' button on the profile model.||Verify that when user clicks the 'OK' button on the Neon on-boarding welcome triggers the display of the Profile modal. || Verify that user who clicks the 'Done' button on the profile modal shall be sent to their desired location in Project Neon.</t>
+  </si>
+  <si>
+    <t>OPQA-2101||OPQA-2100</t>
   </si>
   <si>
     <t xml:space="preserve"> 
-Verify that profile modal displays the profile picture of the user.|Verify that profile modal displays text that explains introduces the profile concept.</t>
-  </si>
-  <si>
-    <t>Profile58</t>
-  </si>
-  <si>
-    <t>OPQA-2105|OPQA-2103</t>
-  </si>
-  <si>
-    <t>Verify that user has the ability to update his Name from the profile modal.|Verify that profile modal displays the following fields pre-populated with values from the user's profile:Name (required field),Title/Role,Country,Skills and Interests (Topics)</t>
-  </si>
-  <si>
-    <t>Profile59</t>
-  </si>
-  <si>
-    <t>OPQA-2108</t>
-  </si>
-  <si>
-    <t>Verify that user has the ability to add and update the following information from the profile modal:Title/Role,Institution,Country,Skills and Interests (Topics)</t>
-  </si>
-  <si>
-    <t>Profile60</t>
-  </si>
-  <si>
-    <t>OPQA-2096</t>
-  </si>
-  <si>
-    <t>Verify that the system records the user as on-boarded if he exits the Neon on-boarding welcome modal without clicking on the "Done" button.</t>
-  </si>
-  <si>
-    <t>Profile61</t>
-  </si>
-  <si>
-    <t>OPQA-2087</t>
-  </si>
-  <si>
-    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Project Neon" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
-  </si>
-  <si>
-    <t>OPQA-2089</t>
-  </si>
-  <si>
-    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Profile" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
-  </si>
-  <si>
-    <t>Profile62</t>
-  </si>
-  <si>
-    <t>OPQA-2090</t>
-  </si>
-  <si>
-    <t>Verify that ENW user who has not been on-boarded to Neon when clicks on "Account" link from within ENW, shall be presented with the Neon on-boarding welcome modal.</t>
-  </si>
-  <si>
-    <t>Profile63</t>
-  </si>
-  <si>
-    <t>Profile64</t>
-  </si>
-  <si>
-    <t>OPQA-1722</t>
-  </si>
-  <si>
-    <t>Verify that  A signed in ENW user shall be able to try to access their Feedback page via a link within the ENW header profile dropdown</t>
-  </si>
-  <si>
-    <t>Profile65</t>
-  </si>
-  <si>
-    <t>Profile66</t>
-  </si>
-  <si>
-    <t>OPQA-1715</t>
-  </si>
-  <si>
-    <t>Verify that  A signed in ENW user shall be able to try to access their Privacy page via a link within the ENW header profile dropdown.</t>
-  </si>
-  <si>
-    <t>OPQA-1718</t>
-  </si>
-  <si>
-    <t>Verify that  A signed in ENW user shall be able to try to access their Acceptable Use page via a link within the ENW header profile dropdown</t>
+Verify that profile modal displays the profile picture of the user.||Verify that profile modal displays text that explains introduces the profile concept.</t>
+  </si>
+  <si>
+    <t>OPQA-2105||OPQA-2103</t>
+  </si>
+  <si>
+    <t>Verify that user has the ability to update his Name from the profile modal.||Verify that profile modal displays the following fields pre-populated with values from the user's profile:Name (required field),Title/Role,Country,Skills and Interests (Topics)</t>
   </si>
 </sst>
 </file>
@@ -844,7 +844,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -857,9 +857,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -885,6 +882,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1187,16 +1196,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="173.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="110.5703125" style="21" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1205,9 +1214,9 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1219,1073 +1228,1073 @@
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>194</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="75">
       <c r="A8" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="90">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30">
       <c r="A13" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
       <c r="A15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>42</v>
+        <v>101</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>44</v>
+        <v>102</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>46</v>
+        <v>103</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>49</v>
+        <v>104</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>52</v>
+        <v>105</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>55</v>
+        <v>106</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>107</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>57</v>
+        <v>108</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>58</v>
+        <v>109</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>63</v>
+        <v>110</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>64</v>
+        <v>111</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>65</v>
+        <v>112</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>66</v>
+        <v>113</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>67</v>
+        <v>114</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>68</v>
+        <v>115</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>69</v>
+        <v>116</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>70</v>
+        <v>117</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>71</v>
+        <v>118</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>72</v>
+        <v>119</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>73</v>
+        <v>120</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>74</v>
+        <v>121</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>130</v>
+      <c r="B43" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>135</v>
+        <v>128</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5" ht="45">
+        <v>46</v>
+      </c>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" ht="60">
       <c r="A45" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="8"/>
+        <v>131</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" ht="30">
+      <c r="A47" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="30">
+      <c r="A48" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" s="13"/>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B49" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" t="s">
-        <v>146</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E48" s="14"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="8"/>
+        <v>147</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>156</v>
+        <v>148</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E51" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>159</v>
+        <v>151</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>152</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E52" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" s="8"/>
+        <v>153</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" spans="1:5" ht="30">
+        <v>46</v>
+      </c>
+      <c r="E54" s="7"/>
+    </row>
+    <row r="55" spans="1:5" ht="45">
       <c r="A55" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="8"/>
+        <v>159</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:5" ht="45">
+      <c r="A57" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:5" ht="45">
+      <c r="A58" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="1:5" ht="45">
+      <c r="A59" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B59" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5" ht="30">
-      <c r="A57" s="2" t="s">
+      <c r="C60" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="D60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C61" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="D57" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:5" ht="30">
-      <c r="A58" s="2" t="s">
+      <c r="D61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="D62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5" ht="30">
-      <c r="A59" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B59" s="19" t="s">
+      <c r="D63" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="1:5" ht="30">
+      <c r="A64" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C64" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B60" s="8" t="s">
+      <c r="D64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="1:5" ht="30">
+      <c r="A65" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="8"/>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="2" t="s">
+      <c r="C65" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="D65" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="1:5" ht="30">
+      <c r="A66" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="B66" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" spans="1:5" ht="30">
+      <c r="A67" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D61" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C62" s="8" t="s">
+      <c r="B67" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B63" s="8" t="s">
+      <c r="C67" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E63" s="8"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E65" s="8"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D66" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E67" s="8"/>
+      <c r="D67" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
profile script code changes to remove skips
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="204">
   <si>
     <t>TCID</t>
   </si>
@@ -162,9 +162,6 @@
     <t xml:space="preserve">Verify that user is able to see all his POST's from his profile page. </t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
   </si>
   <si>
     <t>OPQA-515</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>Verify that user is able to add 'primary institution' using type ahead</t>
@@ -1196,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1206,7 +1200,7 @@
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="110.5703125" style="21" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1228,41 +1222,37 @@
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>33</v>
@@ -1271,15 +1261,13 @@
         <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>36</v>
@@ -1288,32 +1276,28 @@
         <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>15</v>
@@ -1322,32 +1306,28 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="75">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="90">
       <c r="A9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -1356,15 +1336,13 @@
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
@@ -1373,15 +1351,13 @@
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="30">
       <c r="A11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>17</v>
@@ -1390,32 +1366,28 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" ht="30">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
@@ -1424,15 +1396,13 @@
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>20</v>
@@ -1441,15 +1411,13 @@
         <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="30">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>22</v>
@@ -1458,15 +1426,13 @@
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>23</v>
@@ -1475,15 +1441,13 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>24</v>
@@ -1492,15 +1456,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
@@ -1509,15 +1471,13 @@
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>26</v>
@@ -1526,15 +1486,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>27</v>
@@ -1543,15 +1501,13 @@
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>38</v>
@@ -1560,15 +1516,13 @@
         <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>40</v>
@@ -1577,15 +1531,13 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>42</v>
@@ -1594,15 +1546,13 @@
         <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>43</v>
@@ -1611,688 +1561,652 @@
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>49</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="C42" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" ht="60">
       <c r="A45" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>134</v>
-      </c>
       <c r="C46" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" ht="30">
       <c r="A47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="C47" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>140</v>
-      </c>
       <c r="C48" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E48" s="13"/>
     </row>
     <row r="49" spans="1:5" ht="30">
       <c r="A49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>152</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="45">
       <c r="A55" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>162</v>
-      </c>
       <c r="D56" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="45">
       <c r="A57" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C57" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>165</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="45">
       <c r="A58" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" ht="45">
       <c r="A59" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>170</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>173</v>
-      </c>
       <c r="D61" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>176</v>
-      </c>
       <c r="D62" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" ht="30">
       <c r="A65" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>185</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="30">
       <c r="A66" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="C66" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" ht="30">
       <c r="A67" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E67" s="7"/>
     </row>

</xml_diff>

<commit_message>
profile onboarding modals script fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -580,9 +580,6 @@
     <t>OPQA-2115</t>
   </si>
   <si>
-    <t>Verify that user shall be marked as on-boarded if they exit the profile modal without clicking the 'Done' button.</t>
-  </si>
-  <si>
     <t>Profile56</t>
   </si>
   <si>
@@ -611,9 +608,6 @@
   </si>
   <si>
     <t>OPQA-2096</t>
-  </si>
-  <si>
-    <t>Verify that the system records the user as on-boarded if he exits the Neon on-boarding welcome modal without clicking on the "Done" button.</t>
   </si>
   <si>
     <t>Profile61</t>
@@ -699,9 +693,6 @@
     <t>OPQA-2116||OPQA-2094||OPQA-2112</t>
   </si>
   <si>
-    <t>Verify that user shall be marked as on-boarded if they click the 'Done' button on the profile model.||Verify that when user clicks the 'OK' button on the Neon on-boarding welcome triggers the display of the Profile modal. || Verify that user who clicks the 'Done' button on the profile modal shall be sent to their desired location in Project Neon.</t>
-  </si>
-  <si>
     <t>OPQA-2101||OPQA-2100</t>
   </si>
   <si>
@@ -731,6 +722,15 @@
   </si>
   <si>
     <t>Verify that when user clicks outside of the profile model then user will be sent right to their desired location in Neon.</t>
+  </si>
+  <si>
+    <t>Verify that user shall be marked as non on-boarded if they exit the profile modal without clicking the 'Join' button.</t>
+  </si>
+  <si>
+    <t>Verify that the system records the user as non on-boarded if he exits the Neon on-boarding welcome modal without clicking on the "Next" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user shall be marked as on-boarded if they click the 'Join' button on the profile model.||Verify that when user clicks the 'Next' button on the Neon on-boarding welcome triggers the display of the Profile modal. || Verify that user who clicks the 'Join' button on the profile modal shall be sent to their desired location in Project Neon. </t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1243,10 +1243,10 @@
         <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>45</v>
@@ -1258,7 +1258,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
@@ -1303,7 +1303,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -1393,7 +1393,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
@@ -1888,10 +1888,10 @@
         <v>129</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>194</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>196</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>45</v>
@@ -1978,7 +1978,7 @@
         <v>146</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>147</v>
@@ -2038,10 +2038,10 @@
         <v>157</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>45</v>
@@ -2056,7 +2056,7 @@
         <v>159</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>45</v>
@@ -2065,13 +2065,13 @@
     </row>
     <row r="57" spans="1:5" ht="45">
       <c r="A57" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="17" t="s">
         <v>162</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>163</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>45</v>
@@ -2080,13 +2080,13 @@
     </row>
     <row r="58" spans="1:5" ht="45">
       <c r="A58" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>45</v>
@@ -2095,13 +2095,13 @@
     </row>
     <row r="59" spans="1:5" ht="45">
       <c r="A59" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>45</v>
@@ -2110,13 +2110,13 @@
     </row>
     <row r="60" spans="1:5" ht="30">
       <c r="A60" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="C60" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>45</v>
@@ -2125,13 +2125,13 @@
     </row>
     <row r="61" spans="1:5" ht="30">
       <c r="A61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>170</v>
-      </c>
       <c r="C61" s="11" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>45</v>
@@ -2140,13 +2140,13 @@
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>45</v>
@@ -2155,13 +2155,13 @@
     </row>
     <row r="63" spans="1:5" ht="30">
       <c r="A63" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>45</v>
@@ -2170,13 +2170,13 @@
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>45</v>
@@ -2185,13 +2185,13 @@
     </row>
     <row r="65" spans="1:5" ht="30">
       <c r="A65" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C65" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>45</v>
@@ -2200,13 +2200,13 @@
     </row>
     <row r="66" spans="1:5" ht="30">
       <c r="A66" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="C66" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>45</v>
@@ -2215,13 +2215,13 @@
     </row>
     <row r="67" spans="1:5" ht="30">
       <c r="A67" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>45</v>
@@ -2230,13 +2230,13 @@
     </row>
     <row r="68" spans="1:5" ht="30">
       <c r="A68" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>45</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="C69" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Profile image upload script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="213">
   <si>
     <t>TCID</t>
   </si>
@@ -731,6 +731,15 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that user shall be marked as on-boarded if they click the 'Join' button on the profile model.||Verify that when user clicks the 'Next' button on the Neon on-boarding welcome triggers the display of the Profile modal. || Verify that user who clicks the 'Join' button on the profile modal shall be sent to their desired location in Project Neon. </t>
+  </si>
+  <si>
+    <t>Profile69</t>
+  </si>
+  <si>
+    <t>OPQA-500</t>
+  </si>
+  <si>
+    <t>Verify that user is able to update his own profile picture</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2258,6 +2267,21 @@
       </c>
       <c r="E69" s="7"/>
     </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B42" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2726"/>

</xml_diff>

<commit_message>
new script added for profile
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="222">
   <si>
     <t>TCID</t>
   </si>
@@ -744,9 +744,6 @@
     <t>Profile71</t>
   </si>
   <si>
-    <t>OPQA-TBD</t>
-  </si>
-  <si>
     <t>Verify that First time logged user Profile tabs should display with default messags for each tab and count should be '0'</t>
   </si>
   <si>
@@ -754,6 +751,18 @@
   </si>
   <si>
     <t>Verify that app should open in a second window, when user clicks on the "Go" button next to BAU app</t>
+  </si>
+  <si>
+    <t>Profile72</t>
+  </si>
+  <si>
+    <t>Verify that Watchlist tab infinite scroll displaying the more available records</t>
+  </si>
+  <si>
+    <t>OPQA-4820</t>
+  </si>
+  <si>
+    <t>OPQA-4821</t>
   </si>
 </sst>
 </file>
@@ -1229,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1356,10 +1365,10 @@
         <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>44</v>
@@ -2316,15 +2325,30 @@
         <v>214</v>
       </c>
       <c r="B72" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C72" s="11" t="s">
-        <v>216</v>
-      </c>
       <c r="D72" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E72" s="7"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E73" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
changed runmode to N due to functionality not available
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Profile.xlsx
+++ b/src/test/resources/xls/Profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="224">
   <si>
     <t>TCID</t>
   </si>
@@ -763,6 +763,12 @@
   </si>
   <si>
     <t>OPQA-4821</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Setting Runmode Status is 'N' due to functionality got disabled timebeing, enable once its back</t>
   </si>
 </sst>
 </file>
@@ -844,7 +850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -880,6 +886,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -888,7 +905,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -938,6 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1238,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1253,7 +1271,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="2" t="s">
         <v>79</v>
       </c>
@@ -1285,7 +1303,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="2" t="s">
         <v>80</v>
       </c>
@@ -1300,7 +1318,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1315,7 +1333,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
@@ -1330,7 +1348,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="2" t="s">
         <v>83</v>
       </c>
@@ -1345,7 +1363,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>84</v>
       </c>
@@ -1360,7 +1378,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>85</v>
       </c>
@@ -1371,11 +1389,14 @@
         <v>217</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="90">
+      <c r="F8" s="23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90">
       <c r="A9" s="2" t="s">
         <v>86</v>
       </c>
@@ -1390,7 +1411,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="2" t="s">
         <v>87</v>
       </c>
@@ -1405,7 +1426,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="2" t="s">
         <v>88</v>
       </c>
@@ -1420,7 +1441,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>89</v>
       </c>
@@ -1435,7 +1456,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="2" t="s">
         <v>90</v>
       </c>
@@ -1450,7 +1471,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
@@ -1465,7 +1486,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
@@ -1480,7 +1501,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>93</v>
       </c>

</xml_diff>